<commit_message>
fetch materials with course object
</commit_message>
<xml_diff>
--- a/APIs.xlsx
+++ b/APIs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="57">
   <si>
     <t>Module</t>
   </si>
@@ -206,9 +206,6 @@
   </si>
   <si>
     <t>http://localhost:3000/courses/getByStd/:id</t>
-  </si>
-  <si>
-    <t>http://localhost:3000/courses/enrollments</t>
   </si>
   <si>
     <t>http://localhost:3000/courses/tags</t>
@@ -663,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F47"/>
+  <dimension ref="A2:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -868,7 +865,7 @@
         <v>5</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -898,10 +895,10 @@
         <v>9</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -909,29 +906,29 @@
         <v>9</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="3" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
         <v>36</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>38</v>
@@ -939,10 +936,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>39</v>
@@ -950,10 +947,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>40</v>
@@ -961,10 +958,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>41</v>
@@ -972,7 +969,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>5</v>
@@ -981,23 +978,23 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="3" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
         <v>43</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>45</v>
@@ -1005,10 +1002,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>46</v>
@@ -1016,10 +1013,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>47</v>
@@ -1027,10 +1024,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>48</v>
@@ -1038,7 +1035,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>5</v>
@@ -1047,23 +1044,23 @@
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="3" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>50</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>52</v>
@@ -1071,10 +1068,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>53</v>
@@ -1082,10 +1079,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>54</v>
@@ -1093,10 +1090,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>55</v>
@@ -1104,24 +1101,13 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1142,28 +1128,27 @@
     <hyperlink ref="C20" r:id="rId14"/>
     <hyperlink ref="C21" r:id="rId15"/>
     <hyperlink ref="C22" r:id="rId16"/>
-    <hyperlink ref="C23" r:id="rId17"/>
+    <hyperlink ref="C25" r:id="rId17"/>
     <hyperlink ref="C26" r:id="rId18"/>
     <hyperlink ref="C27" r:id="rId19"/>
     <hyperlink ref="C28" r:id="rId20"/>
     <hyperlink ref="C29" r:id="rId21"/>
     <hyperlink ref="C30" r:id="rId22"/>
-    <hyperlink ref="C31" r:id="rId23"/>
+    <hyperlink ref="C33" r:id="rId23"/>
     <hyperlink ref="C34" r:id="rId24"/>
     <hyperlink ref="C35" r:id="rId25"/>
     <hyperlink ref="C36" r:id="rId26"/>
     <hyperlink ref="C37" r:id="rId27"/>
     <hyperlink ref="C38" r:id="rId28"/>
-    <hyperlink ref="C39" r:id="rId29"/>
+    <hyperlink ref="C41" r:id="rId29"/>
     <hyperlink ref="C42" r:id="rId30"/>
     <hyperlink ref="C43" r:id="rId31"/>
     <hyperlink ref="C44" r:id="rId32"/>
     <hyperlink ref="C45" r:id="rId33"/>
     <hyperlink ref="C46" r:id="rId34"/>
-    <hyperlink ref="C47" r:id="rId35"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId36"/>
+  <pageSetup orientation="portrait" r:id="rId35"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
forgot password for App
</commit_message>
<xml_diff>
--- a/APIs.xlsx
+++ b/APIs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="89">
   <si>
     <t>Module</t>
   </si>
@@ -226,17 +226,11 @@
     <t>To get the encrypted string of the given password</t>
   </si>
   <si>
-    <t>http://localhost:3000/users/forgotPass</t>
-  </si>
-  <si>
     <t>{
 "username":"hardiskbohra@gmail.com"
 }</t>
   </si>
   <si>
-    <t>To get the password change link on mail when you forgot the password</t>
-  </si>
-  <si>
     <t>http://localhost:3000/users/changePassword</t>
   </si>
   <si>
@@ -304,6 +298,18 @@
   </si>
   <si>
     <t>http://localhost:3000/announcements/delete/:id</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/users/web/forgotPass</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/users/app/forgotPass</t>
+  </si>
+  <si>
+    <t>To get the password change link on mail when you click on forgot password from web</t>
+  </si>
+  <si>
+    <t>To get the password change link on mail when you click on forgot password from app</t>
   </si>
 </sst>
 </file>
@@ -683,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F59"/>
+  <dimension ref="A2:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -843,13 +849,13 @@
         <v>6</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -857,55 +863,58 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="C13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C13" s="3"/>
+      <c r="E13" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+      <c r="C14" s="3"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>68</v>
-      </c>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -916,10 +925,10 @@
         <v>6</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -927,13 +936,13 @@
         <v>9</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -941,30 +950,30 @@
         <v>9</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>9</v>
       </c>
@@ -972,13 +981,13 @@
         <v>5</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>9</v>
       </c>
@@ -986,10 +995,10 @@
         <v>5</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1000,13 +1009,13 @@
         <v>5</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>66</v>
+        <v>23</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>9</v>
       </c>
@@ -1014,10 +1023,10 @@
         <v>5</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1025,13 +1034,13 @@
         <v>9</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1039,24 +1048,27 @@
         <v>9</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>29</v>
+      <c r="E28" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1064,10 +1076,10 @@
         <v>28</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1075,10 +1087,10 @@
         <v>28</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -1086,10 +1098,10 @@
         <v>28</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -1097,10 +1109,10 @@
         <v>28</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -1111,18 +1123,18 @@
         <v>5</v>
       </c>
       <c r="C35" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -1130,10 +1142,10 @@
         <v>35</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -1141,10 +1153,10 @@
         <v>35</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -1152,10 +1164,10 @@
         <v>35</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -1163,10 +1175,10 @@
         <v>35</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -1177,18 +1189,18 @@
         <v>5</v>
       </c>
       <c r="C43" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -1196,10 +1208,10 @@
         <v>42</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -1207,10 +1219,10 @@
         <v>42</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -1218,10 +1230,10 @@
         <v>42</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -1229,10 +1241,10 @@
         <v>42</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -1243,73 +1255,85 @@
         <v>5</v>
       </c>
       <c r="C51" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
+    <row r="54" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C59" s="3" t="s">
-        <v>86</v>
+      <c r="C60" s="3" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1320,48 +1344,49 @@
     <hyperlink ref="C9" r:id="rId4"/>
     <hyperlink ref="C5" r:id="rId5"/>
     <hyperlink ref="C7" r:id="rId6"/>
-    <hyperlink ref="C16" r:id="rId7"/>
-    <hyperlink ref="C18" r:id="rId8"/>
-    <hyperlink ref="C19" r:id="rId9"/>
-    <hyperlink ref="C20" r:id="rId10"/>
-    <hyperlink ref="C21" r:id="rId11"/>
-    <hyperlink ref="C22" r:id="rId12"/>
-    <hyperlink ref="C24" r:id="rId13"/>
-    <hyperlink ref="C25" r:id="rId14"/>
-    <hyperlink ref="C26" r:id="rId15"/>
-    <hyperlink ref="C27" r:id="rId16"/>
-    <hyperlink ref="C30" r:id="rId17"/>
-    <hyperlink ref="C31" r:id="rId18"/>
-    <hyperlink ref="C32" r:id="rId19"/>
-    <hyperlink ref="C33" r:id="rId20"/>
-    <hyperlink ref="C34" r:id="rId21"/>
-    <hyperlink ref="C35" r:id="rId22"/>
-    <hyperlink ref="C38" r:id="rId23"/>
-    <hyperlink ref="C39" r:id="rId24"/>
-    <hyperlink ref="C40" r:id="rId25"/>
-    <hyperlink ref="C41" r:id="rId26"/>
-    <hyperlink ref="C42" r:id="rId27"/>
-    <hyperlink ref="C43" r:id="rId28"/>
-    <hyperlink ref="C46" r:id="rId29"/>
-    <hyperlink ref="C47" r:id="rId30"/>
-    <hyperlink ref="C48" r:id="rId31"/>
-    <hyperlink ref="C49" r:id="rId32"/>
-    <hyperlink ref="C50" r:id="rId33"/>
-    <hyperlink ref="C51" r:id="rId34"/>
+    <hyperlink ref="C17" r:id="rId7"/>
+    <hyperlink ref="C19" r:id="rId8"/>
+    <hyperlink ref="C20" r:id="rId9"/>
+    <hyperlink ref="C21" r:id="rId10"/>
+    <hyperlink ref="C22" r:id="rId11"/>
+    <hyperlink ref="C23" r:id="rId12"/>
+    <hyperlink ref="C25" r:id="rId13"/>
+    <hyperlink ref="C26" r:id="rId14"/>
+    <hyperlink ref="C27" r:id="rId15"/>
+    <hyperlink ref="C28" r:id="rId16"/>
+    <hyperlink ref="C31" r:id="rId17"/>
+    <hyperlink ref="C32" r:id="rId18"/>
+    <hyperlink ref="C33" r:id="rId19"/>
+    <hyperlink ref="C34" r:id="rId20"/>
+    <hyperlink ref="C35" r:id="rId21"/>
+    <hyperlink ref="C36" r:id="rId22"/>
+    <hyperlink ref="C39" r:id="rId23"/>
+    <hyperlink ref="C40" r:id="rId24"/>
+    <hyperlink ref="C41" r:id="rId25"/>
+    <hyperlink ref="C42" r:id="rId26"/>
+    <hyperlink ref="C43" r:id="rId27"/>
+    <hyperlink ref="C44" r:id="rId28"/>
+    <hyperlink ref="C47" r:id="rId29"/>
+    <hyperlink ref="C48" r:id="rId30"/>
+    <hyperlink ref="C49" r:id="rId31"/>
+    <hyperlink ref="C50" r:id="rId32"/>
+    <hyperlink ref="C51" r:id="rId33"/>
+    <hyperlink ref="C52" r:id="rId34"/>
     <hyperlink ref="C10" r:id="rId35"/>
     <hyperlink ref="C11" r:id="rId36"/>
-    <hyperlink ref="C12" r:id="rId37"/>
-    <hyperlink ref="C23" r:id="rId38"/>
-    <hyperlink ref="C17" r:id="rId39"/>
-    <hyperlink ref="C54" r:id="rId40"/>
-    <hyperlink ref="C55" r:id="rId41"/>
-    <hyperlink ref="C56" r:id="rId42"/>
-    <hyperlink ref="C57" r:id="rId43"/>
-    <hyperlink ref="C58" r:id="rId44"/>
-    <hyperlink ref="C59" r:id="rId45"/>
+    <hyperlink ref="C24" r:id="rId37"/>
+    <hyperlink ref="C18" r:id="rId38"/>
+    <hyperlink ref="C55" r:id="rId39"/>
+    <hyperlink ref="C56" r:id="rId40"/>
+    <hyperlink ref="C57" r:id="rId41"/>
+    <hyperlink ref="C58" r:id="rId42"/>
+    <hyperlink ref="C59" r:id="rId43"/>
+    <hyperlink ref="C60" r:id="rId44"/>
+    <hyperlink ref="C13" r:id="rId45"/>
+    <hyperlink ref="C12" r:id="rId46"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId46"/>
+  <pageSetup orientation="portrait" r:id="rId47"/>
 </worksheet>
 </file>
 

</xml_diff>